<commit_message>
update data and call for contribution
</commit_message>
<xml_diff>
--- a/data/垃圾运输.xlsx
+++ b/data/垃圾运输.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wangge/Mygithub/Vehicle-LCA-economy/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDBC861A-6AFE-A246-AA90-ECCCDAC44A0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C75736DB-3CE9-7143-B68A-83A7B7B6584E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="20920" windowHeight="9660" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="燃油汽车" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="71">
   <si>
     <t>单位</t>
   </si>
@@ -81,30 +81,12 @@
     <t>百公里能耗</t>
   </si>
   <si>
-    <t>燃料价格</t>
-  </si>
-  <si>
-    <t>元/L</t>
-  </si>
-  <si>
     <t>低温能耗率</t>
   </si>
   <si>
     <t>-</t>
   </si>
   <si>
-    <t>充能速度</t>
-  </si>
-  <si>
-    <t>L/小时</t>
-  </si>
-  <si>
-    <t>燃料生命周期排放因子</t>
-  </si>
-  <si>
-    <t>kgCO2/L</t>
-  </si>
-  <si>
     <t>保养费用</t>
   </si>
   <si>
@@ -150,9 +132,6 @@
     <t>车身单位成本</t>
   </si>
   <si>
-    <t>元/kwh</t>
-  </si>
-  <si>
     <t>电池容量</t>
   </si>
   <si>
@@ -162,12 +141,6 @@
     <t>kg/kwh</t>
   </si>
   <si>
-    <t>kWh/小时</t>
-  </si>
-  <si>
-    <t>kgCO2/kWh</t>
-  </si>
-  <si>
     <t>燃料电池系统功率</t>
   </si>
   <si>
@@ -186,12 +159,6 @@
     <t>元/kg</t>
   </si>
   <si>
-    <t>kg/小时</t>
-  </si>
-  <si>
-    <t>kgCO2/kg</t>
-  </si>
-  <si>
     <t>折现率</t>
   </si>
   <si>
@@ -283,7 +250,7 @@
   </si>
   <si>
     <t>否</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -293,7 +260,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0.00_ "/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -337,12 +304,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FFEBB07A"/>
-      <name val="Menlo"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="9"/>
       <name val="等线"/>
       <family val="4"/>
@@ -366,7 +327,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -401,15 +362,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color indexed="64"/>
@@ -428,7 +380,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -465,16 +417,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -752,10 +698,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P18"/>
+  <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10:L10"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="R16" sqref="R16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -763,7 +709,7 @@
     <col min="1" max="1" width="19.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:12">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -797,20 +743,8 @@
       <c r="L1" s="3">
         <v>2030</v>
       </c>
-      <c r="M1" s="3">
-        <v>2031</v>
-      </c>
-      <c r="N1" s="3">
-        <v>2032</v>
-      </c>
-      <c r="O1" s="3">
-        <v>2033</v>
-      </c>
-      <c r="P1" s="3">
-        <v>2034</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16">
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -847,12 +781,8 @@
       <c r="L2" s="8">
         <v>160583.44570433401</v>
       </c>
-      <c r="M2" s="8"/>
-      <c r="N2" s="8"/>
-      <c r="O2" s="8"/>
-      <c r="P2" s="8"/>
-    </row>
-    <row r="3" spans="1:16">
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
@@ -889,12 +819,8 @@
       <c r="L3" s="8">
         <v>131839.420229893</v>
       </c>
-      <c r="M3" s="8"/>
-      <c r="N3" s="8"/>
-      <c r="O3" s="8"/>
-      <c r="P3" s="8"/>
-    </row>
-    <row r="4" spans="1:16">
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -931,12 +857,8 @@
       <c r="L4" s="8">
         <v>400</v>
       </c>
-      <c r="M4" s="8"/>
-      <c r="N4" s="8"/>
-      <c r="O4" s="8"/>
-      <c r="P4" s="8"/>
-    </row>
-    <row r="5" spans="1:16">
+    </row>
+    <row r="5" spans="1:12">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -973,12 +895,8 @@
       <c r="L5" s="8">
         <v>13000</v>
       </c>
-      <c r="M5" s="8"/>
-      <c r="N5" s="8"/>
-      <c r="O5" s="8"/>
-      <c r="P5" s="8"/>
-    </row>
-    <row r="6" spans="1:16">
+    </row>
+    <row r="6" spans="1:12">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -1015,12 +933,8 @@
       <c r="L6" s="4">
         <v>0</v>
       </c>
-      <c r="M6" s="4"/>
-      <c r="N6" s="4"/>
-      <c r="O6" s="4"/>
-      <c r="P6" s="4"/>
-    </row>
-    <row r="7" spans="1:16">
+    </row>
+    <row r="7" spans="1:12">
       <c r="A7" s="3" t="s">
         <v>9</v>
       </c>
@@ -1067,12 +981,8 @@
         <f t="shared" si="0"/>
         <v>65000</v>
       </c>
-      <c r="M7" s="8"/>
-      <c r="N7" s="8"/>
-      <c r="O7" s="8"/>
-      <c r="P7" s="8"/>
-    </row>
-    <row r="8" spans="1:16">
+    </row>
+    <row r="8" spans="1:12">
       <c r="A8" s="9" t="s">
         <v>10</v>
       </c>
@@ -1119,12 +1029,8 @@
         <f t="shared" si="1"/>
         <v>357422.86593422701</v>
       </c>
-      <c r="M8" s="10"/>
-      <c r="N8" s="10"/>
-      <c r="O8" s="10"/>
-      <c r="P8" s="10"/>
-    </row>
-    <row r="9" spans="1:16">
+    </row>
+    <row r="9" spans="1:12">
       <c r="A9" s="9" t="s">
         <v>11</v>
       </c>
@@ -1161,12 +1067,8 @@
       <c r="L9" s="10">
         <v>63775.382891914</v>
       </c>
-      <c r="M9" s="10"/>
-      <c r="N9" s="10"/>
-      <c r="O9" s="10"/>
-      <c r="P9" s="10"/>
-    </row>
-    <row r="10" spans="1:16">
+    </row>
+    <row r="10" spans="1:12">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
@@ -1213,12 +1115,8 @@
         <f t="shared" si="2"/>
         <v>421198.248826141</v>
       </c>
-      <c r="M10" s="10"/>
-      <c r="N10" s="10"/>
-      <c r="O10" s="10"/>
-      <c r="P10" s="10"/>
-    </row>
-    <row r="11" spans="1:16">
+    </row>
+    <row r="11" spans="1:12">
       <c r="A11" s="1" t="s">
         <v>13</v>
       </c>
@@ -1255,360 +1153,198 @@
       <c r="L11" s="4">
         <v>59.196091111240598</v>
       </c>
-      <c r="M11" s="4"/>
-      <c r="N11" s="4"/>
-      <c r="O11" s="4"/>
-      <c r="P11" s="4"/>
-    </row>
-    <row r="12" spans="1:16">
+    </row>
+    <row r="12" spans="1:12">
       <c r="A12" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="3">
-        <v>8.1449999999999996</v>
-      </c>
-      <c r="D12" s="3">
-        <v>8.1449999999999996</v>
-      </c>
-      <c r="E12" s="3">
-        <v>8.1449999999999996</v>
-      </c>
-      <c r="F12" s="3">
-        <v>8.1449999999999996</v>
-      </c>
-      <c r="G12" s="3">
-        <v>8.1449999999999996</v>
-      </c>
-      <c r="H12" s="3">
-        <v>8.1449999999999996</v>
-      </c>
-      <c r="I12" s="3">
-        <v>8.1449999999999996</v>
-      </c>
-      <c r="J12" s="3">
-        <v>8.1449999999999996</v>
-      </c>
-      <c r="K12" s="3">
-        <v>8.1449999999999996</v>
-      </c>
-      <c r="L12" s="3">
-        <v>8.1449999999999996</v>
-      </c>
-      <c r="M12" s="3">
-        <v>8.1449999999999996</v>
-      </c>
-      <c r="N12" s="3">
-        <v>8.1449999999999996</v>
-      </c>
-      <c r="O12" s="3">
-        <v>8.1449999999999996</v>
-      </c>
-      <c r="P12" s="3">
-        <v>8.1449999999999996</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16">
-      <c r="A13" s="1" t="s">
+      <c r="C12" s="6">
+        <v>1</v>
+      </c>
+      <c r="D12" s="6">
+        <v>1</v>
+      </c>
+      <c r="E12" s="6">
+        <v>1</v>
+      </c>
+      <c r="F12" s="6">
+        <v>1</v>
+      </c>
+      <c r="G12" s="6">
+        <v>1</v>
+      </c>
+      <c r="H12" s="6">
+        <v>1</v>
+      </c>
+      <c r="I12" s="6">
+        <v>1</v>
+      </c>
+      <c r="J12" s="6">
+        <v>1</v>
+      </c>
+      <c r="K12" s="6">
+        <v>1</v>
+      </c>
+      <c r="L12" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B13" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="6">
-        <v>1</v>
-      </c>
-      <c r="D13" s="6">
-        <v>1</v>
-      </c>
-      <c r="E13" s="6">
-        <v>1</v>
-      </c>
-      <c r="F13" s="6">
-        <v>1</v>
-      </c>
-      <c r="G13" s="6">
-        <v>1</v>
-      </c>
-      <c r="H13" s="6">
-        <v>1</v>
-      </c>
-      <c r="I13" s="6">
-        <v>1</v>
-      </c>
-      <c r="J13" s="6">
-        <v>1</v>
-      </c>
-      <c r="K13" s="6">
-        <v>1</v>
-      </c>
-      <c r="L13" s="6">
-        <v>1</v>
-      </c>
-      <c r="M13" s="6"/>
-      <c r="N13" s="6"/>
-      <c r="O13" s="6"/>
-      <c r="P13" s="6"/>
-    </row>
-    <row r="14" spans="1:16">
+      <c r="C13" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="D13" s="5">
+        <f t="shared" ref="D13:L13" si="3">C13</f>
+        <v>0.2</v>
+      </c>
+      <c r="E13" s="5">
+        <f t="shared" si="3"/>
+        <v>0.2</v>
+      </c>
+      <c r="F13" s="5">
+        <f t="shared" si="3"/>
+        <v>0.2</v>
+      </c>
+      <c r="G13" s="5">
+        <f t="shared" si="3"/>
+        <v>0.2</v>
+      </c>
+      <c r="H13" s="5">
+        <f t="shared" si="3"/>
+        <v>0.2</v>
+      </c>
+      <c r="I13" s="5">
+        <f t="shared" si="3"/>
+        <v>0.2</v>
+      </c>
+      <c r="J13" s="5">
+        <f t="shared" si="3"/>
+        <v>0.2</v>
+      </c>
+      <c r="K13" s="5">
+        <f t="shared" si="3"/>
+        <v>0.2</v>
+      </c>
+      <c r="L13" s="5">
+        <f t="shared" si="3"/>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
       <c r="A14" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="12">
-        <v>6000</v>
-      </c>
-      <c r="D14" s="12">
-        <v>6000</v>
-      </c>
-      <c r="E14" s="12">
-        <v>6000</v>
-      </c>
-      <c r="F14" s="12">
-        <v>6000</v>
-      </c>
-      <c r="G14" s="12">
-        <v>6000</v>
-      </c>
-      <c r="H14" s="12">
-        <v>6000</v>
-      </c>
-      <c r="I14" s="12">
-        <v>6000</v>
-      </c>
-      <c r="J14" s="12">
-        <v>6000</v>
-      </c>
-      <c r="K14" s="12">
-        <v>6000</v>
-      </c>
-      <c r="L14" s="12">
-        <v>6000</v>
-      </c>
-      <c r="M14" s="12"/>
-      <c r="N14" s="12"/>
-      <c r="O14" s="12"/>
-      <c r="P14" s="12"/>
-    </row>
-    <row r="15" spans="1:16">
+      <c r="C14" s="4">
+        <v>5000</v>
+      </c>
+      <c r="D14" s="5">
+        <f t="shared" ref="D14:L14" si="4">C14</f>
+        <v>5000</v>
+      </c>
+      <c r="E14" s="5">
+        <f t="shared" si="4"/>
+        <v>5000</v>
+      </c>
+      <c r="F14" s="5">
+        <f t="shared" si="4"/>
+        <v>5000</v>
+      </c>
+      <c r="G14" s="5">
+        <f t="shared" si="4"/>
+        <v>5000</v>
+      </c>
+      <c r="H14" s="5">
+        <f t="shared" si="4"/>
+        <v>5000</v>
+      </c>
+      <c r="I14" s="5">
+        <f t="shared" si="4"/>
+        <v>5000</v>
+      </c>
+      <c r="J14" s="5">
+        <f t="shared" si="4"/>
+        <v>5000</v>
+      </c>
+      <c r="K14" s="5">
+        <f t="shared" si="4"/>
+        <v>5000</v>
+      </c>
+      <c r="L14" s="5">
+        <f t="shared" si="4"/>
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
       <c r="A15" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C15" s="12">
-        <v>2.63</v>
-      </c>
-      <c r="D15" s="12">
-        <v>2.63</v>
-      </c>
-      <c r="E15" s="12">
-        <v>2.63</v>
-      </c>
-      <c r="F15" s="12">
-        <v>2.63</v>
-      </c>
-      <c r="G15" s="12">
-        <v>2.63</v>
-      </c>
-      <c r="H15" s="12">
-        <v>2.63</v>
-      </c>
-      <c r="I15" s="12">
-        <v>2.63</v>
-      </c>
-      <c r="J15" s="12">
-        <v>2.63</v>
-      </c>
-      <c r="K15" s="12">
-        <v>2.63</v>
-      </c>
-      <c r="L15" s="12">
-        <v>2.63</v>
-      </c>
-      <c r="M15" s="12">
-        <v>2.63</v>
-      </c>
-      <c r="N15" s="12">
-        <v>2.63</v>
-      </c>
-      <c r="O15" s="12">
-        <v>2.63</v>
-      </c>
-      <c r="P15" s="12">
-        <v>2.63</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16">
-      <c r="A16" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B16" t="s">
-        <v>23</v>
-      </c>
-      <c r="C16" s="4">
-        <v>0.2</v>
-      </c>
-      <c r="D16" s="5">
-        <f t="shared" ref="D16:L16" si="3">C16</f>
-        <v>0.2</v>
-      </c>
-      <c r="E16" s="5">
-        <f t="shared" si="3"/>
-        <v>0.2</v>
-      </c>
-      <c r="F16" s="5">
-        <f t="shared" si="3"/>
-        <v>0.2</v>
-      </c>
-      <c r="G16" s="5">
-        <f t="shared" si="3"/>
-        <v>0.2</v>
-      </c>
-      <c r="H16" s="5">
-        <f t="shared" si="3"/>
-        <v>0.2</v>
-      </c>
-      <c r="I16" s="5">
-        <f t="shared" si="3"/>
-        <v>0.2</v>
-      </c>
-      <c r="J16" s="5">
-        <f t="shared" si="3"/>
-        <v>0.2</v>
-      </c>
-      <c r="K16" s="5">
-        <f t="shared" si="3"/>
-        <v>0.2</v>
-      </c>
-      <c r="L16" s="5">
-        <f t="shared" si="3"/>
-        <v>0.2</v>
-      </c>
-      <c r="M16" s="5"/>
-      <c r="N16" s="5"/>
-      <c r="O16" s="5"/>
-      <c r="P16" s="5"/>
-    </row>
-    <row r="17" spans="1:16">
-      <c r="A17" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="B17" t="s">
-        <v>25</v>
-      </c>
-      <c r="C17" s="4">
-        <v>5000</v>
-      </c>
-      <c r="D17" s="5">
-        <f t="shared" ref="D17:L17" si="4">C17</f>
-        <v>5000</v>
-      </c>
-      <c r="E17" s="5">
-        <f t="shared" si="4"/>
-        <v>5000</v>
-      </c>
-      <c r="F17" s="5">
-        <f t="shared" si="4"/>
-        <v>5000</v>
-      </c>
-      <c r="G17" s="5">
-        <f t="shared" si="4"/>
-        <v>5000</v>
-      </c>
-      <c r="H17" s="5">
-        <f t="shared" si="4"/>
-        <v>5000</v>
-      </c>
-      <c r="I17" s="5">
-        <f t="shared" si="4"/>
-        <v>5000</v>
-      </c>
-      <c r="J17" s="5">
-        <f t="shared" si="4"/>
-        <v>5000</v>
-      </c>
-      <c r="K17" s="5">
-        <f t="shared" si="4"/>
-        <v>5000</v>
-      </c>
-      <c r="L17" s="5">
-        <f t="shared" si="4"/>
-        <v>5000</v>
-      </c>
-      <c r="M17" s="5"/>
-      <c r="N17" s="5"/>
-      <c r="O17" s="5"/>
-      <c r="P17" s="5"/>
-    </row>
-    <row r="18" spans="1:16">
-      <c r="A18" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="B18" t="s">
-        <v>25</v>
-      </c>
-      <c r="C18" s="4">
+      <c r="B15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="4">
         <v>2000</v>
       </c>
-      <c r="D18" s="5">
-        <f t="shared" ref="D18:L18" si="5">C18</f>
+      <c r="D15" s="5">
+        <f t="shared" ref="D15:L15" si="5">C15</f>
         <v>2000</v>
       </c>
-      <c r="E18" s="5">
+      <c r="E15" s="5">
         <f t="shared" si="5"/>
         <v>2000</v>
       </c>
-      <c r="F18" s="5">
+      <c r="F15" s="5">
         <f t="shared" si="5"/>
         <v>2000</v>
       </c>
-      <c r="G18" s="5">
+      <c r="G15" s="5">
         <f t="shared" si="5"/>
         <v>2000</v>
       </c>
-      <c r="H18" s="5">
+      <c r="H15" s="5">
         <f t="shared" si="5"/>
         <v>2000</v>
       </c>
-      <c r="I18" s="5">
+      <c r="I15" s="5">
         <f t="shared" si="5"/>
         <v>2000</v>
       </c>
-      <c r="J18" s="5">
+      <c r="J15" s="5">
         <f t="shared" si="5"/>
         <v>2000</v>
       </c>
-      <c r="K18" s="5">
+      <c r="K15" s="5">
         <f t="shared" si="5"/>
         <v>2000</v>
       </c>
-      <c r="L18" s="5">
+      <c r="L15" s="5">
         <f t="shared" si="5"/>
         <v>2000</v>
       </c>
-      <c r="M18" s="5"/>
-      <c r="N18" s="5"/>
-      <c r="O18" s="5"/>
-      <c r="P18" s="5"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:P22"/>
+  <dimension ref="A1:L19"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13:P13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -1616,7 +1352,7 @@
     <col min="1" max="1" width="21.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:12">
       <c r="A1" s="3"/>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -1651,25 +1387,13 @@
       <c r="L1" s="3">
         <v>2030</v>
       </c>
-      <c r="M1" s="3">
-        <v>2031</v>
-      </c>
-      <c r="N1" s="3">
-        <v>2032</v>
-      </c>
-      <c r="O1" s="3">
-        <v>2033</v>
-      </c>
-      <c r="P1" s="3">
-        <v>2034</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16">
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C2" s="8">
         <v>420</v>
@@ -1701,17 +1425,13 @@
       <c r="L2" s="8">
         <v>420</v>
       </c>
-      <c r="M2" s="8"/>
-      <c r="N2" s="8"/>
-      <c r="O2" s="8"/>
-      <c r="P2" s="8"/>
-    </row>
-    <row r="3" spans="1:16">
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3" s="3" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C3" s="8">
         <v>900</v>
@@ -1743,17 +1463,13 @@
       <c r="L3" s="8">
         <v>433.90523863231101</v>
       </c>
-      <c r="M3" s="8"/>
-      <c r="N3" s="8"/>
-      <c r="O3" s="8"/>
-      <c r="P3" s="8"/>
-    </row>
-    <row r="4" spans="1:16">
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4" s="3" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C4" s="8">
         <v>200</v>
@@ -1785,17 +1501,13 @@
       <c r="L4" s="8">
         <v>200</v>
       </c>
-      <c r="M4" s="8"/>
-      <c r="N4" s="8"/>
-      <c r="O4" s="8"/>
-      <c r="P4" s="8"/>
-    </row>
-    <row r="5" spans="1:16">
+    </row>
+    <row r="5" spans="1:12">
       <c r="A5" s="3" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C5" s="8">
         <v>1000</v>
@@ -1827,17 +1539,13 @@
       <c r="L5" s="8">
         <v>869.20871515059002</v>
       </c>
-      <c r="M5" s="8"/>
-      <c r="N5" s="8"/>
-      <c r="O5" s="8"/>
-      <c r="P5" s="8"/>
-    </row>
-    <row r="6" spans="1:16">
+    </row>
+    <row r="6" spans="1:12">
       <c r="A6" s="3" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C6" s="8">
         <v>2</v>
@@ -1869,12 +1577,8 @@
       <c r="L6" s="8">
         <v>2</v>
       </c>
-      <c r="M6" s="4"/>
-      <c r="N6" s="4"/>
-      <c r="O6" s="4"/>
-      <c r="P6" s="4"/>
-    </row>
-    <row r="7" spans="1:16">
+    </row>
+    <row r="7" spans="1:12">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -1911,14 +1615,10 @@
       <c r="L7" s="8">
         <v>13000</v>
       </c>
-      <c r="M7" s="8"/>
-      <c r="N7" s="8"/>
-      <c r="O7" s="8"/>
-      <c r="P7" s="8"/>
-    </row>
-    <row r="8" spans="1:16">
+    </row>
+    <row r="8" spans="1:12">
       <c r="A8" s="3" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>2</v>
@@ -1953,12 +1653,8 @@
       <c r="L8" s="8">
         <v>5</v>
       </c>
-      <c r="M8" s="10"/>
-      <c r="N8" s="10"/>
-      <c r="O8" s="10"/>
-      <c r="P8" s="10"/>
-    </row>
-    <row r="9" spans="1:16">
+    </row>
+    <row r="9" spans="1:12">
       <c r="A9" s="9" t="s">
         <v>10</v>
       </c>
@@ -2005,12 +1701,8 @@
         <f t="shared" si="0"/>
         <v>594923.68628580659</v>
       </c>
-      <c r="M9" s="10"/>
-      <c r="N9" s="10"/>
-      <c r="O9" s="10"/>
-      <c r="P9" s="10"/>
-    </row>
-    <row r="10" spans="1:16">
+    </row>
+    <row r="10" spans="1:12">
       <c r="A10" s="9" t="s">
         <v>11</v>
       </c>
@@ -2047,12 +1739,8 @@
       <c r="L10" s="10">
         <v>56464.079025541701</v>
       </c>
-      <c r="M10" s="10"/>
-      <c r="N10" s="10"/>
-      <c r="O10" s="10"/>
-      <c r="P10" s="10"/>
-    </row>
-    <row r="11" spans="1:16">
+    </row>
+    <row r="11" spans="1:12">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
@@ -2099,17 +1787,13 @@
         <f t="shared" si="1"/>
         <v>651387.76531134825</v>
       </c>
-      <c r="M11" s="4"/>
-      <c r="N11" s="4"/>
-      <c r="O11" s="4"/>
-      <c r="P11" s="4"/>
-    </row>
-    <row r="12" spans="1:16">
+    </row>
+    <row r="12" spans="1:12">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C12" s="4">
         <v>200</v>
@@ -2141,478 +1825,312 @@
       <c r="L12" s="4">
         <v>166.74955242602999</v>
       </c>
-      <c r="M12" s="4"/>
-      <c r="N12" s="4"/>
-      <c r="O12" s="4"/>
-      <c r="P12" s="4"/>
-    </row>
-    <row r="13" spans="1:16">
-      <c r="A13" s="1" t="s">
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="8">
+        <v>420</v>
+      </c>
+      <c r="D13" s="8">
+        <v>420</v>
+      </c>
+      <c r="E13" s="8">
+        <v>420</v>
+      </c>
+      <c r="F13" s="8">
+        <v>420</v>
+      </c>
+      <c r="G13" s="8">
+        <v>420</v>
+      </c>
+      <c r="H13" s="8">
+        <v>420</v>
+      </c>
+      <c r="I13" s="8">
+        <v>420</v>
+      </c>
+      <c r="J13" s="8">
+        <v>420</v>
+      </c>
+      <c r="K13" s="8">
+        <v>420</v>
+      </c>
+      <c r="L13" s="8">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="4">
+        <v>6.2111801242236</v>
+      </c>
+      <c r="D14" s="4">
+        <v>6.1490683229813703</v>
+      </c>
+      <c r="E14" s="4">
+        <v>6.0881987577639798</v>
+      </c>
+      <c r="F14" s="4">
+        <v>6.02853416149068</v>
+      </c>
+      <c r="G14" s="4">
+        <v>5.9700387577639704</v>
+      </c>
+      <c r="H14" s="4">
+        <v>5.9126781863354001</v>
+      </c>
+      <c r="I14" s="4">
+        <v>5.85641943304348</v>
+      </c>
+      <c r="J14" s="4">
+        <v>5.80123076391056</v>
+      </c>
+      <c r="K14" s="4">
+        <v>5.7470816631107597</v>
+      </c>
+      <c r="L14" s="4">
+        <v>5.69394277454363</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="4">
+        <v>2608.6956521739098</v>
+      </c>
+      <c r="D15" s="4">
+        <v>2582.6086956521799</v>
+      </c>
+      <c r="E15" s="4">
+        <v>2557.04347826087</v>
+      </c>
+      <c r="F15" s="4">
+        <v>2531.98434782609</v>
+      </c>
+      <c r="G15" s="4">
+        <v>2507.4162782608701</v>
+      </c>
+      <c r="H15" s="4">
+        <v>2483.3248382608699</v>
+      </c>
+      <c r="I15" s="4">
+        <v>2459.6961618782602</v>
+      </c>
+      <c r="J15" s="4">
+        <v>2436.51692084244</v>
+      </c>
+      <c r="K15" s="4">
+        <v>2413.7742985065202</v>
+      </c>
+      <c r="L15" s="4">
+        <v>2391.4559653083202</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C13" s="3">
-        <v>0.9</v>
-      </c>
-      <c r="D13" s="3">
-        <v>0.9</v>
-      </c>
-      <c r="E13" s="3">
-        <v>0.9</v>
-      </c>
-      <c r="F13" s="3">
-        <v>0.9</v>
-      </c>
-      <c r="G13" s="3">
-        <v>0.9</v>
-      </c>
-      <c r="H13" s="3">
-        <v>0.9</v>
-      </c>
-      <c r="I13" s="3">
-        <v>0.9</v>
-      </c>
-      <c r="J13" s="3">
-        <v>0.9</v>
-      </c>
-      <c r="K13" s="3">
-        <v>0.9</v>
-      </c>
-      <c r="L13" s="3">
-        <v>0.9</v>
-      </c>
-      <c r="M13" s="6">
-        <f>L13</f>
-        <v>0.9</v>
-      </c>
-      <c r="N13" s="6">
-        <f>M13</f>
-        <v>0.9</v>
-      </c>
-      <c r="O13" s="6">
-        <f>N13</f>
-        <v>0.9</v>
-      </c>
-      <c r="P13" s="6">
-        <f>O13</f>
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16">
-      <c r="A14" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C14" s="8">
-        <v>420</v>
-      </c>
-      <c r="D14" s="8">
-        <v>420</v>
-      </c>
-      <c r="E14" s="8">
-        <v>420</v>
-      </c>
-      <c r="F14" s="8">
-        <v>420</v>
-      </c>
-      <c r="G14" s="8">
-        <v>420</v>
-      </c>
-      <c r="H14" s="8">
-        <v>420</v>
-      </c>
-      <c r="I14" s="8">
-        <v>420</v>
-      </c>
-      <c r="J14" s="8">
-        <v>420</v>
-      </c>
-      <c r="K14" s="8">
-        <v>420</v>
-      </c>
-      <c r="L14" s="8">
-        <v>420</v>
-      </c>
-      <c r="M14" s="12"/>
-      <c r="N14" s="12"/>
-      <c r="O14" s="12"/>
-      <c r="P14" s="12"/>
-    </row>
-    <row r="15" spans="1:16">
-      <c r="A15" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C15" s="4">
-        <v>6.2111801242236</v>
-      </c>
-      <c r="D15" s="4">
-        <v>6.1490683229813703</v>
-      </c>
-      <c r="E15" s="4">
-        <v>6.0881987577639798</v>
-      </c>
-      <c r="F15" s="4">
-        <v>6.02853416149068</v>
-      </c>
-      <c r="G15" s="4">
-        <v>5.9700387577639704</v>
-      </c>
-      <c r="H15" s="4">
-        <v>5.9126781863354001</v>
-      </c>
-      <c r="I15" s="4">
-        <v>5.85641943304348</v>
-      </c>
-      <c r="J15" s="4">
-        <v>5.80123076391056</v>
-      </c>
-      <c r="K15" s="4">
-        <v>5.7470816631107597</v>
-      </c>
-      <c r="L15" s="4">
-        <v>5.69394277454363</v>
-      </c>
-      <c r="M15" s="12"/>
-      <c r="N15" s="12"/>
-      <c r="O15" s="12"/>
-      <c r="P15" s="12"/>
-    </row>
-    <row r="16" spans="1:16">
-      <c r="A16" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C16" s="4">
-        <v>2608.6956521739098</v>
-      </c>
-      <c r="D16" s="4">
-        <v>2582.6086956521799</v>
-      </c>
-      <c r="E16" s="4">
-        <v>2557.04347826087</v>
-      </c>
-      <c r="F16" s="4">
-        <v>2531.98434782609</v>
-      </c>
-      <c r="G16" s="4">
-        <v>2507.4162782608701</v>
-      </c>
-      <c r="H16" s="4">
-        <v>2483.3248382608699</v>
-      </c>
-      <c r="I16" s="4">
-        <v>2459.6961618782602</v>
-      </c>
-      <c r="J16" s="4">
-        <v>2436.51692084244</v>
-      </c>
-      <c r="K16" s="4">
-        <v>2413.7742985065202</v>
-      </c>
-      <c r="L16" s="4">
-        <v>2391.4559653083202</v>
-      </c>
-      <c r="M16" s="5"/>
-      <c r="N16" s="5"/>
-      <c r="O16" s="5"/>
-      <c r="P16" s="5"/>
-    </row>
-    <row r="17" spans="1:16">
-      <c r="A17" s="1" t="s">
+      <c r="B16" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="6">
+        <v>2</v>
+      </c>
+      <c r="D16" s="6">
+        <v>2</v>
+      </c>
+      <c r="E16" s="6">
+        <v>2</v>
+      </c>
+      <c r="F16" s="6">
+        <v>2</v>
+      </c>
+      <c r="G16" s="6">
+        <v>2</v>
+      </c>
+      <c r="H16" s="6">
+        <v>2</v>
+      </c>
+      <c r="I16" s="6">
+        <v>2</v>
+      </c>
+      <c r="J16" s="6">
+        <v>2</v>
+      </c>
+      <c r="K16" s="6">
+        <v>2</v>
+      </c>
+      <c r="L16" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="A17" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="B17" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="6">
-        <v>2</v>
-      </c>
-      <c r="D17" s="6">
-        <v>2</v>
-      </c>
-      <c r="E17" s="6">
-        <v>2</v>
-      </c>
-      <c r="F17" s="6">
-        <v>2</v>
-      </c>
-      <c r="G17" s="6">
-        <v>2</v>
-      </c>
-      <c r="H17" s="6">
-        <v>2</v>
-      </c>
-      <c r="I17" s="6">
-        <v>2</v>
-      </c>
-      <c r="J17" s="6">
-        <v>2</v>
-      </c>
-      <c r="K17" s="6">
-        <v>2</v>
-      </c>
-      <c r="L17" s="6">
-        <v>2</v>
-      </c>
-      <c r="M17" s="5"/>
-      <c r="N17" s="5"/>
-      <c r="O17" s="5"/>
-      <c r="P17" s="5"/>
-    </row>
-    <row r="18" spans="1:16">
+      <c r="C17" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="D17" s="5">
+        <f t="shared" ref="D17:L17" si="2">C17</f>
+        <v>0.2</v>
+      </c>
+      <c r="E17" s="5">
+        <f t="shared" si="2"/>
+        <v>0.2</v>
+      </c>
+      <c r="F17" s="5">
+        <f t="shared" si="2"/>
+        <v>0.2</v>
+      </c>
+      <c r="G17" s="5">
+        <f t="shared" si="2"/>
+        <v>0.2</v>
+      </c>
+      <c r="H17" s="5">
+        <f t="shared" si="2"/>
+        <v>0.2</v>
+      </c>
+      <c r="I17" s="5">
+        <f t="shared" si="2"/>
+        <v>0.2</v>
+      </c>
+      <c r="J17" s="5">
+        <f t="shared" si="2"/>
+        <v>0.2</v>
+      </c>
+      <c r="K17" s="5">
+        <f t="shared" si="2"/>
+        <v>0.2</v>
+      </c>
+      <c r="L17" s="5">
+        <f t="shared" si="2"/>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
       <c r="A18" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="C18" s="12">
-        <v>250</v>
-      </c>
-      <c r="D18" s="12">
-        <v>250</v>
-      </c>
-      <c r="E18" s="12">
-        <v>250</v>
-      </c>
-      <c r="F18" s="12">
-        <v>250</v>
-      </c>
-      <c r="G18" s="12">
-        <v>250</v>
-      </c>
-      <c r="H18" s="12">
-        <v>250</v>
-      </c>
-      <c r="I18" s="12">
-        <v>250</v>
-      </c>
-      <c r="J18" s="12">
-        <v>250</v>
-      </c>
-      <c r="K18" s="12">
-        <v>250</v>
-      </c>
-      <c r="L18" s="12">
-        <v>250</v>
-      </c>
-      <c r="M18" s="5"/>
-      <c r="N18" s="5"/>
-      <c r="O18" s="5"/>
-      <c r="P18" s="5"/>
-    </row>
-    <row r="19" spans="1:16">
+      <c r="B18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="4">
+        <v>5000</v>
+      </c>
+      <c r="D18" s="5">
+        <f t="shared" ref="D18:L18" si="3">C18</f>
+        <v>5000</v>
+      </c>
+      <c r="E18" s="5">
+        <f t="shared" si="3"/>
+        <v>5000</v>
+      </c>
+      <c r="F18" s="5">
+        <f t="shared" si="3"/>
+        <v>5000</v>
+      </c>
+      <c r="G18" s="5">
+        <f t="shared" si="3"/>
+        <v>5000</v>
+      </c>
+      <c r="H18" s="5">
+        <f t="shared" si="3"/>
+        <v>5000</v>
+      </c>
+      <c r="I18" s="5">
+        <f t="shared" si="3"/>
+        <v>5000</v>
+      </c>
+      <c r="J18" s="5">
+        <f t="shared" si="3"/>
+        <v>5000</v>
+      </c>
+      <c r="K18" s="5">
+        <f t="shared" si="3"/>
+        <v>5000</v>
+      </c>
+      <c r="L18" s="5">
+        <f t="shared" si="3"/>
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
       <c r="A19" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="C19" s="13">
-        <v>0.56499999999999995</v>
-      </c>
-      <c r="D19" s="12">
-        <v>0.57030000000000003</v>
-      </c>
-      <c r="E19" s="12">
-        <v>0.57030000000000003</v>
-      </c>
-      <c r="F19" s="12">
-        <v>0.57030000000000003</v>
-      </c>
-      <c r="G19" s="12">
-        <v>0.57030000000000003</v>
-      </c>
-      <c r="H19" s="12">
-        <v>0.57030000000000003</v>
-      </c>
-      <c r="I19" s="12">
-        <v>0.57030000000000003</v>
-      </c>
-      <c r="J19" s="12">
-        <v>0.57030000000000003</v>
-      </c>
-      <c r="K19" s="12">
-        <v>0.57030000000000003</v>
-      </c>
-      <c r="L19" s="12">
-        <v>0.57030000000000003</v>
-      </c>
-      <c r="M19" s="12">
-        <v>0.57030000000000003</v>
-      </c>
-      <c r="N19" s="12">
-        <v>0.57030000000000003</v>
-      </c>
-      <c r="O19" s="12">
-        <v>0.57030000000000003</v>
-      </c>
-      <c r="P19" s="12">
-        <v>0.57030000000000003</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16">
-      <c r="A20" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B20" t="s">
-        <v>23</v>
-      </c>
-      <c r="C20" s="4">
-        <v>0.2</v>
-      </c>
-      <c r="D20" s="5">
-        <f t="shared" ref="D20:L20" si="2">C20</f>
-        <v>0.2</v>
-      </c>
-      <c r="E20" s="5">
-        <f t="shared" si="2"/>
-        <v>0.2</v>
-      </c>
-      <c r="F20" s="5">
-        <f t="shared" si="2"/>
-        <v>0.2</v>
-      </c>
-      <c r="G20" s="5">
-        <f t="shared" si="2"/>
-        <v>0.2</v>
-      </c>
-      <c r="H20" s="5">
-        <f t="shared" si="2"/>
-        <v>0.2</v>
-      </c>
-      <c r="I20" s="5">
-        <f t="shared" si="2"/>
-        <v>0.2</v>
-      </c>
-      <c r="J20" s="5">
-        <f t="shared" si="2"/>
-        <v>0.2</v>
-      </c>
-      <c r="K20" s="5">
-        <f t="shared" si="2"/>
-        <v>0.2</v>
-      </c>
-      <c r="L20" s="5">
-        <f t="shared" si="2"/>
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16">
-      <c r="A21" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="B21" t="s">
-        <v>25</v>
-      </c>
-      <c r="C21" s="4">
-        <v>5000</v>
-      </c>
-      <c r="D21" s="5">
-        <f t="shared" ref="D21:L21" si="3">C21</f>
-        <v>5000</v>
-      </c>
-      <c r="E21" s="5">
-        <f t="shared" si="3"/>
-        <v>5000</v>
-      </c>
-      <c r="F21" s="5">
-        <f t="shared" si="3"/>
-        <v>5000</v>
-      </c>
-      <c r="G21" s="5">
-        <f t="shared" si="3"/>
-        <v>5000</v>
-      </c>
-      <c r="H21" s="5">
-        <f t="shared" si="3"/>
-        <v>5000</v>
-      </c>
-      <c r="I21" s="5">
-        <f t="shared" si="3"/>
-        <v>5000</v>
-      </c>
-      <c r="J21" s="5">
-        <f t="shared" si="3"/>
-        <v>5000</v>
-      </c>
-      <c r="K21" s="5">
-        <f t="shared" si="3"/>
-        <v>5000</v>
-      </c>
-      <c r="L21" s="5">
-        <f t="shared" si="3"/>
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16">
-      <c r="A22" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="B22" t="s">
-        <v>25</v>
-      </c>
-      <c r="C22" s="4">
+      <c r="B19" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="4">
         <v>2000</v>
       </c>
-      <c r="D22" s="5">
-        <f t="shared" ref="D22:L22" si="4">C22</f>
+      <c r="D19" s="5">
+        <f t="shared" ref="D19:L19" si="4">C19</f>
         <v>2000</v>
       </c>
-      <c r="E22" s="5">
+      <c r="E19" s="5">
         <f t="shared" si="4"/>
         <v>2000</v>
       </c>
-      <c r="F22" s="5">
+      <c r="F19" s="5">
         <f t="shared" si="4"/>
         <v>2000</v>
       </c>
-      <c r="G22" s="5">
+      <c r="G19" s="5">
         <f t="shared" si="4"/>
         <v>2000</v>
       </c>
-      <c r="H22" s="5">
+      <c r="H19" s="5">
         <f t="shared" si="4"/>
         <v>2000</v>
       </c>
-      <c r="I22" s="5">
+      <c r="I19" s="5">
         <f t="shared" si="4"/>
         <v>2000</v>
       </c>
-      <c r="J22" s="5">
+      <c r="J19" s="5">
         <f t="shared" si="4"/>
         <v>2000</v>
       </c>
-      <c r="K22" s="5">
+      <c r="K19" s="5">
         <f t="shared" si="4"/>
         <v>2000</v>
       </c>
-      <c r="L22" s="5">
+      <c r="L19" s="5">
         <f t="shared" si="4"/>
         <v>2000</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:P26"/>
+  <dimension ref="A1:L23"/>
   <sheetViews>
-    <sheetView topLeftCell="E7" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17:P17"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -2620,7 +2138,7 @@
     <col min="1" max="1" width="21.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:12">
       <c r="A1" s="3"/>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -2655,25 +2173,13 @@
       <c r="L1" s="3">
         <v>2030</v>
       </c>
-      <c r="M1" s="3">
-        <v>2031</v>
-      </c>
-      <c r="N1" s="3">
-        <v>2032</v>
-      </c>
-      <c r="O1" s="3">
-        <v>2033</v>
-      </c>
-      <c r="P1" s="3">
-        <v>2034</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16">
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2" s="3" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C2" s="8">
         <v>110</v>
@@ -2705,17 +2211,13 @@
       <c r="L2" s="8">
         <v>110</v>
       </c>
-      <c r="M2" s="8"/>
-      <c r="N2" s="8"/>
-      <c r="O2" s="8"/>
-      <c r="P2" s="8"/>
-    </row>
-    <row r="3" spans="1:16">
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3" s="3" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C3" s="8">
         <v>4500</v>
@@ -2747,17 +2249,13 @@
       <c r="L3" s="8">
         <v>639.95709350887205</v>
       </c>
-      <c r="M3" s="8"/>
-      <c r="N3" s="8"/>
-      <c r="O3" s="8"/>
-      <c r="P3" s="8"/>
-    </row>
-    <row r="4" spans="1:16">
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4" s="3" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C4" s="8">
         <v>100</v>
@@ -2789,17 +2287,13 @@
       <c r="L4" s="8">
         <v>100</v>
       </c>
-      <c r="M4" s="8"/>
-      <c r="N4" s="8"/>
-      <c r="O4" s="8"/>
-      <c r="P4" s="8"/>
-    </row>
-    <row r="5" spans="1:16">
+    </row>
+    <row r="5" spans="1:12">
       <c r="A5" s="3" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C5" s="8">
         <v>900</v>
@@ -2831,17 +2325,13 @@
       <c r="L5" s="8">
         <v>433.90523863231101</v>
       </c>
-      <c r="M5" s="8"/>
-      <c r="N5" s="8"/>
-      <c r="O5" s="8"/>
-      <c r="P5" s="8"/>
-    </row>
-    <row r="6" spans="1:16">
+    </row>
+    <row r="6" spans="1:12">
       <c r="A6" s="3" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C6" s="8">
         <v>200</v>
@@ -2873,17 +2363,13 @@
       <c r="L6" s="8">
         <v>200</v>
       </c>
-      <c r="M6" s="4"/>
-      <c r="N6" s="4"/>
-      <c r="O6" s="4"/>
-      <c r="P6" s="4"/>
-    </row>
-    <row r="7" spans="1:16">
+    </row>
+    <row r="7" spans="1:12">
       <c r="A7" s="3" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C7" s="8">
         <v>1000</v>
@@ -2915,17 +2401,13 @@
       <c r="L7" s="8">
         <v>869.20871515059002</v>
       </c>
-      <c r="M7" s="8"/>
-      <c r="N7" s="8"/>
-      <c r="O7" s="8"/>
-      <c r="P7" s="8"/>
-    </row>
-    <row r="8" spans="1:16">
+    </row>
+    <row r="8" spans="1:12">
       <c r="A8" s="3" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C8" s="8">
         <v>2</v>
@@ -2957,12 +2439,8 @@
       <c r="L8" s="8">
         <v>2</v>
       </c>
-      <c r="M8" s="10"/>
-      <c r="N8" s="10"/>
-      <c r="O8" s="10"/>
-      <c r="P8" s="10"/>
-    </row>
-    <row r="9" spans="1:16">
+    </row>
+    <row r="9" spans="1:12">
       <c r="A9" s="1" t="s">
         <v>4</v>
       </c>
@@ -2999,17 +2477,13 @@
       <c r="L9" s="8">
         <v>50</v>
       </c>
-      <c r="M9" s="10"/>
-      <c r="N9" s="10"/>
-      <c r="O9" s="10"/>
-      <c r="P9" s="10"/>
-    </row>
-    <row r="10" spans="1:16">
+    </row>
+    <row r="10" spans="1:12">
       <c r="A10" s="3" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="C10" s="8">
         <v>4900</v>
@@ -3041,12 +2515,8 @@
       <c r="L10" s="8">
         <v>991.98582317815305</v>
       </c>
-      <c r="M10" s="10"/>
-      <c r="N10" s="10"/>
-      <c r="O10" s="10"/>
-      <c r="P10" s="10"/>
-    </row>
-    <row r="11" spans="1:16">
+    </row>
+    <row r="11" spans="1:12">
       <c r="A11" s="1" t="s">
         <v>6</v>
       </c>
@@ -3083,17 +2553,13 @@
       <c r="L11" s="8">
         <v>13000</v>
       </c>
-      <c r="M11" s="4"/>
-      <c r="N11" s="4"/>
-      <c r="O11" s="4"/>
-      <c r="P11" s="4"/>
-    </row>
-    <row r="12" spans="1:16">
+    </row>
+    <row r="12" spans="1:12">
       <c r="A12" s="3" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="C12" s="8">
         <v>5</v>
@@ -3125,24 +2591,8 @@
       <c r="L12" s="8">
         <v>5</v>
       </c>
-      <c r="M12" s="4">
-        <f>L12</f>
-        <v>5</v>
-      </c>
-      <c r="N12" s="4">
-        <f t="shared" ref="N12:P12" si="0">M12</f>
-        <v>5</v>
-      </c>
-      <c r="O12" s="4">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="P12" s="4">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16">
+    </row>
+    <row r="13" spans="1:12">
       <c r="A13" s="9" t="s">
         <v>10</v>
       </c>
@@ -3154,47 +2604,43 @@
         <v>1295000</v>
       </c>
       <c r="D13" s="10">
-        <f t="shared" ref="D13:L13" si="1">D2*D3+D4*D5+D6*D7*D8+D9*D10+D11*D12</f>
+        <f t="shared" ref="D13:L13" si="0">D2*D3+D4*D5+D6*D7*D8+D9*D10+D11*D12</f>
         <v>943493.25018065935</v>
       </c>
       <c r="E13" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>859434.31934236817</v>
       </c>
       <c r="F13" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>824697.35028962535</v>
       </c>
       <c r="G13" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>796551.36044078064</v>
       </c>
       <c r="H13" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>666949.92294671037</v>
       </c>
       <c r="I13" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>619727.56557581923</v>
       </c>
       <c r="J13" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>595328.97672158165</v>
       </c>
       <c r="K13" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>584836.92689352424</v>
       </c>
       <c r="L13" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>576068.58136835066</v>
       </c>
-      <c r="M13" s="6"/>
-      <c r="N13" s="6"/>
-      <c r="O13" s="6"/>
-      <c r="P13" s="6"/>
-    </row>
-    <row r="14" spans="1:16">
+    </row>
+    <row r="14" spans="1:12">
       <c r="A14" s="9" t="s">
         <v>11</v>
       </c>
@@ -3231,12 +2677,8 @@
       <c r="L14" s="10">
         <v>33930.317658677297</v>
       </c>
-      <c r="M14" s="12"/>
-      <c r="N14" s="12"/>
-      <c r="O14" s="12"/>
-      <c r="P14" s="12"/>
-    </row>
-    <row r="15" spans="1:16">
+    </row>
+    <row r="15" spans="1:12">
       <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
@@ -3244,51 +2686,47 @@
         <v>2</v>
       </c>
       <c r="C15" s="10">
-        <f t="shared" ref="C15:L15" si="2">C14+C13</f>
+        <f t="shared" ref="C15:L15" si="1">C14+C13</f>
         <v>1356296.0209078796</v>
       </c>
       <c r="D15" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>991625.63790463796</v>
       </c>
       <c r="E15" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>904285.91524076147</v>
       </c>
       <c r="F15" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>867975.37138324534</v>
       </c>
       <c r="G15" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>838551.41317518696</v>
       </c>
       <c r="H15" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>704362.52948108932</v>
       </c>
       <c r="I15" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>655435.40389893495</v>
       </c>
       <c r="J15" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>630088.25243378361</v>
       </c>
       <c r="K15" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>619133.43855046108</v>
       </c>
       <c r="L15" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>609998.899027028</v>
       </c>
-      <c r="M15" s="12"/>
-      <c r="N15" s="12"/>
-      <c r="O15" s="12"/>
-      <c r="P15" s="12"/>
-    </row>
-    <row r="16" spans="1:16">
+    </row>
+    <row r="16" spans="1:12">
       <c r="A16" s="1" t="s">
         <v>13</v>
       </c>
@@ -3325,452 +2763,302 @@
       <c r="L16" s="4">
         <v>8.3374776213015007</v>
       </c>
-      <c r="M16" s="5"/>
-      <c r="N16" s="5"/>
-      <c r="O16" s="5"/>
-      <c r="P16" s="5"/>
-    </row>
-    <row r="17" spans="1:16">
-      <c r="A17" s="1" t="s">
+    </row>
+    <row r="17" spans="1:12">
+      <c r="A17" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="4">
+        <v>100</v>
+      </c>
+      <c r="D17" s="4">
+        <v>100</v>
+      </c>
+      <c r="E17" s="4">
+        <v>100</v>
+      </c>
+      <c r="F17" s="4">
+        <v>100</v>
+      </c>
+      <c r="G17" s="4">
+        <v>100</v>
+      </c>
+      <c r="H17" s="4">
+        <v>100</v>
+      </c>
+      <c r="I17" s="4">
+        <v>100</v>
+      </c>
+      <c r="J17" s="4">
+        <v>100</v>
+      </c>
+      <c r="K17" s="4">
+        <v>100</v>
+      </c>
+      <c r="L17" s="4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="A18" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" s="4">
+        <v>6.2111801242236</v>
+      </c>
+      <c r="D18" s="4">
+        <v>6.1490683229813703</v>
+      </c>
+      <c r="E18" s="4">
+        <v>6.0881987577639798</v>
+      </c>
+      <c r="F18" s="4">
+        <v>6.02853416149068</v>
+      </c>
+      <c r="G18" s="4">
+        <v>5.9700387577639704</v>
+      </c>
+      <c r="H18" s="4">
+        <v>5.9126781863354001</v>
+      </c>
+      <c r="I18" s="4">
+        <v>5.85641943304348</v>
+      </c>
+      <c r="J18" s="4">
+        <v>5.80123076391056</v>
+      </c>
+      <c r="K18" s="4">
+        <v>5.7470816631107597</v>
+      </c>
+      <c r="L18" s="4">
+        <v>5.69394277454363</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
+      <c r="A19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" s="4">
+        <v>621.11801242236004</v>
+      </c>
+      <c r="D19" s="4">
+        <v>614.90683229813703</v>
+      </c>
+      <c r="E19" s="4">
+        <v>608.81987577639802</v>
+      </c>
+      <c r="F19" s="4">
+        <v>602.85341614906804</v>
+      </c>
+      <c r="G19" s="4">
+        <v>597.00387577639697</v>
+      </c>
+      <c r="H19" s="4">
+        <v>591.26781863353995</v>
+      </c>
+      <c r="I19" s="4">
+        <v>585.64194330434805</v>
+      </c>
+      <c r="J19" s="4">
+        <v>580.12307639105597</v>
+      </c>
+      <c r="K19" s="4">
+        <v>574.70816631107596</v>
+      </c>
+      <c r="L19" s="4">
+        <v>569.39427745436296</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
+      <c r="A20" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C17" s="4">
-        <v>50</v>
-      </c>
-      <c r="D17" s="4">
-        <v>49</v>
-      </c>
-      <c r="E17" s="4">
-        <v>48</v>
-      </c>
-      <c r="F17" s="4">
-        <v>47</v>
-      </c>
-      <c r="G17" s="4">
-        <v>46</v>
-      </c>
-      <c r="H17" s="4">
-        <v>45</v>
-      </c>
-      <c r="I17" s="4">
-        <v>44</v>
-      </c>
-      <c r="J17" s="4">
-        <v>43</v>
-      </c>
-      <c r="K17" s="4">
-        <v>42</v>
-      </c>
-      <c r="L17" s="4">
-        <v>41</v>
-      </c>
-      <c r="M17" s="5">
-        <f>L17-1</f>
-        <v>40</v>
-      </c>
-      <c r="N17" s="5">
-        <f>M17-1</f>
-        <v>39</v>
-      </c>
-      <c r="O17" s="5">
-        <f>N17-1</f>
-        <v>38</v>
-      </c>
-      <c r="P17" s="5">
-        <f>O17-1</f>
-        <v>37</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16">
-      <c r="A18" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C18" s="4">
-        <v>100</v>
-      </c>
-      <c r="D18" s="4">
-        <v>100</v>
-      </c>
-      <c r="E18" s="4">
-        <v>100</v>
-      </c>
-      <c r="F18" s="4">
-        <v>100</v>
-      </c>
-      <c r="G18" s="4">
-        <v>100</v>
-      </c>
-      <c r="H18" s="4">
-        <v>100</v>
-      </c>
-      <c r="I18" s="4">
-        <v>100</v>
-      </c>
-      <c r="J18" s="4">
-        <v>100</v>
-      </c>
-      <c r="K18" s="4">
-        <v>100</v>
-      </c>
-      <c r="L18" s="4">
-        <v>100</v>
-      </c>
-      <c r="M18" s="5"/>
-      <c r="N18" s="5"/>
-      <c r="O18" s="5"/>
-      <c r="P18" s="5"/>
-    </row>
-    <row r="19" spans="1:16">
-      <c r="A19" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C19" s="4">
-        <v>6.2111801242236</v>
-      </c>
-      <c r="D19" s="4">
-        <v>6.1490683229813703</v>
-      </c>
-      <c r="E19" s="4">
-        <v>6.0881987577639798</v>
-      </c>
-      <c r="F19" s="4">
-        <v>6.02853416149068</v>
-      </c>
-      <c r="G19" s="4">
-        <v>5.9700387577639704</v>
-      </c>
-      <c r="H19" s="4">
-        <v>5.9126781863354001</v>
-      </c>
-      <c r="I19" s="4">
-        <v>5.85641943304348</v>
-      </c>
-      <c r="J19" s="4">
-        <v>5.80123076391056</v>
-      </c>
-      <c r="K19" s="4">
-        <v>5.7470816631107597</v>
-      </c>
-      <c r="L19" s="4">
-        <v>5.69394277454363</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16">
-      <c r="A20" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C20" s="4">
-        <v>621.11801242236004</v>
-      </c>
-      <c r="D20" s="4">
-        <v>614.90683229813703</v>
-      </c>
-      <c r="E20" s="4">
-        <v>608.81987577639802</v>
-      </c>
-      <c r="F20" s="4">
-        <v>602.85341614906804</v>
-      </c>
-      <c r="G20" s="4">
-        <v>597.00387577639697</v>
-      </c>
-      <c r="H20" s="4">
-        <v>591.26781863353995</v>
-      </c>
-      <c r="I20" s="4">
-        <v>585.64194330434805</v>
-      </c>
-      <c r="J20" s="4">
-        <v>580.12307639105597</v>
-      </c>
-      <c r="K20" s="4">
-        <v>574.70816631107596</v>
-      </c>
-      <c r="L20" s="4">
-        <v>569.39427745436296</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16">
+      <c r="B20" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="6">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D20" s="6">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E20" s="6">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F20" s="6">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G20" s="6">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H20" s="6">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="I20" s="6">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="J20" s="6">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K20" s="6">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="L20" s="6">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
       <c r="A21" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B21" s="11" t="s">
+      <c r="B21" t="s">
         <v>17</v>
       </c>
-      <c r="C21" s="6">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="D21" s="6">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="E21" s="6">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="F21" s="6">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="G21" s="6">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="H21" s="6">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="I21" s="6">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="J21" s="6">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="K21" s="6">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="L21" s="6">
-        <v>1.1000000000000001</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16">
-      <c r="A22" s="7" t="s">
+      <c r="C21" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="D21" s="5">
+        <f t="shared" ref="D21:L21" si="2">C21</f>
+        <v>0.2</v>
+      </c>
+      <c r="E21" s="5">
+        <f t="shared" si="2"/>
+        <v>0.2</v>
+      </c>
+      <c r="F21" s="5">
+        <f t="shared" si="2"/>
+        <v>0.2</v>
+      </c>
+      <c r="G21" s="5">
+        <f t="shared" si="2"/>
+        <v>0.2</v>
+      </c>
+      <c r="H21" s="5">
+        <f t="shared" si="2"/>
+        <v>0.2</v>
+      </c>
+      <c r="I21" s="5">
+        <f t="shared" si="2"/>
+        <v>0.2</v>
+      </c>
+      <c r="J21" s="5">
+        <f t="shared" si="2"/>
+        <v>0.2</v>
+      </c>
+      <c r="K21" s="5">
+        <f t="shared" si="2"/>
+        <v>0.2</v>
+      </c>
+      <c r="L21" s="5">
+        <f t="shared" si="2"/>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
+      <c r="A22" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B22" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="C22" s="12">
-        <v>500</v>
-      </c>
-      <c r="D22" s="12">
-        <v>500</v>
-      </c>
-      <c r="E22" s="12">
-        <v>500</v>
-      </c>
-      <c r="F22" s="12">
-        <v>500</v>
-      </c>
-      <c r="G22" s="12">
-        <v>500</v>
-      </c>
-      <c r="H22" s="12">
-        <v>500</v>
-      </c>
-      <c r="I22" s="12">
-        <v>500</v>
-      </c>
-      <c r="J22" s="12">
-        <v>500</v>
-      </c>
-      <c r="K22" s="12">
-        <v>500</v>
-      </c>
-      <c r="L22" s="12">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16">
-      <c r="A23" s="7" t="s">
+      <c r="B22" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" s="4">
+        <v>5000</v>
+      </c>
+      <c r="D22" s="5">
+        <f t="shared" ref="D22:L22" si="3">C22</f>
+        <v>5000</v>
+      </c>
+      <c r="E22" s="5">
+        <f t="shared" si="3"/>
+        <v>5000</v>
+      </c>
+      <c r="F22" s="5">
+        <f t="shared" si="3"/>
+        <v>5000</v>
+      </c>
+      <c r="G22" s="5">
+        <f t="shared" si="3"/>
+        <v>5000</v>
+      </c>
+      <c r="H22" s="5">
+        <f t="shared" si="3"/>
+        <v>5000</v>
+      </c>
+      <c r="I22" s="5">
+        <f t="shared" si="3"/>
+        <v>5000</v>
+      </c>
+      <c r="J22" s="5">
+        <f t="shared" si="3"/>
+        <v>5000</v>
+      </c>
+      <c r="K22" s="5">
+        <f t="shared" si="3"/>
+        <v>5000</v>
+      </c>
+      <c r="L22" s="5">
+        <f t="shared" si="3"/>
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
+      <c r="A23" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B23" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="C23" s="13">
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="D23" s="13">
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="E23" s="13">
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="F23" s="13">
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="G23" s="13">
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="H23" s="13">
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="I23" s="13">
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="J23" s="13">
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="K23" s="13">
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="L23" s="13">
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="M23" s="13">
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="N23" s="13">
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="O23" s="13">
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="P23" s="13">
-        <v>4.9000000000000004</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16">
-      <c r="A24" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B24" t="s">
-        <v>23</v>
-      </c>
-      <c r="C24" s="4">
-        <v>0.2</v>
-      </c>
-      <c r="D24" s="5">
-        <f t="shared" ref="D24:L24" si="3">C24</f>
-        <v>0.2</v>
-      </c>
-      <c r="E24" s="5">
-        <f t="shared" si="3"/>
-        <v>0.2</v>
-      </c>
-      <c r="F24" s="5">
-        <f t="shared" si="3"/>
-        <v>0.2</v>
-      </c>
-      <c r="G24" s="5">
-        <f t="shared" si="3"/>
-        <v>0.2</v>
-      </c>
-      <c r="H24" s="5">
-        <f t="shared" si="3"/>
-        <v>0.2</v>
-      </c>
-      <c r="I24" s="5">
-        <f t="shared" si="3"/>
-        <v>0.2</v>
-      </c>
-      <c r="J24" s="5">
-        <f t="shared" si="3"/>
-        <v>0.2</v>
-      </c>
-      <c r="K24" s="5">
-        <f t="shared" si="3"/>
-        <v>0.2</v>
-      </c>
-      <c r="L24" s="5">
-        <f t="shared" si="3"/>
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16">
-      <c r="A25" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B25" t="s">
-        <v>25</v>
-      </c>
-      <c r="C25" s="4">
-        <v>5000</v>
-      </c>
-      <c r="D25" s="5">
-        <f t="shared" ref="D25:L25" si="4">C25</f>
-        <v>5000</v>
-      </c>
-      <c r="E25" s="5">
+      <c r="B23" t="s">
+        <v>19</v>
+      </c>
+      <c r="C23" s="4">
+        <v>2000</v>
+      </c>
+      <c r="D23" s="5">
+        <f t="shared" ref="D23:L23" si="4">C23</f>
+        <v>2000</v>
+      </c>
+      <c r="E23" s="5">
         <f t="shared" si="4"/>
-        <v>5000</v>
-      </c>
-      <c r="F25" s="5">
+        <v>2000</v>
+      </c>
+      <c r="F23" s="5">
         <f t="shared" si="4"/>
-        <v>5000</v>
-      </c>
-      <c r="G25" s="5">
+        <v>2000</v>
+      </c>
+      <c r="G23" s="5">
         <f t="shared" si="4"/>
-        <v>5000</v>
-      </c>
-      <c r="H25" s="5">
+        <v>2000</v>
+      </c>
+      <c r="H23" s="5">
         <f t="shared" si="4"/>
-        <v>5000</v>
-      </c>
-      <c r="I25" s="5">
+        <v>2000</v>
+      </c>
+      <c r="I23" s="5">
         <f t="shared" si="4"/>
-        <v>5000</v>
-      </c>
-      <c r="J25" s="5">
+        <v>2000</v>
+      </c>
+      <c r="J23" s="5">
         <f t="shared" si="4"/>
-        <v>5000</v>
-      </c>
-      <c r="K25" s="5">
+        <v>2000</v>
+      </c>
+      <c r="K23" s="5">
         <f t="shared" si="4"/>
-        <v>5000</v>
-      </c>
-      <c r="L25" s="5">
+        <v>2000</v>
+      </c>
+      <c r="L23" s="5">
         <f t="shared" si="4"/>
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16">
-      <c r="A26" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B26" t="s">
-        <v>25</v>
-      </c>
-      <c r="C26" s="4">
         <v>2000</v>
       </c>
-      <c r="D26" s="5">
-        <f t="shared" ref="D26:L26" si="5">C26</f>
-        <v>2000</v>
-      </c>
-      <c r="E26" s="5">
-        <f t="shared" si="5"/>
-        <v>2000</v>
-      </c>
-      <c r="F26" s="5">
-        <f t="shared" si="5"/>
-        <v>2000</v>
-      </c>
-      <c r="G26" s="5">
-        <f t="shared" si="5"/>
-        <v>2000</v>
-      </c>
-      <c r="H26" s="5">
-        <f t="shared" si="5"/>
-        <v>2000</v>
-      </c>
-      <c r="I26" s="5">
-        <f t="shared" si="5"/>
-        <v>2000</v>
-      </c>
-      <c r="J26" s="5">
-        <f t="shared" si="5"/>
-        <v>2000</v>
-      </c>
-      <c r="K26" s="5">
-        <f t="shared" si="5"/>
-        <v>2000</v>
-      </c>
-      <c r="L26" s="5">
-        <f t="shared" si="5"/>
-        <v>2000</v>
-      </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3779,7 +3067,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
@@ -3826,10 +3114,10 @@
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="1" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C2" s="4">
         <v>0.06</v>
@@ -3873,10 +3161,10 @@
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="1" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="B3" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="C3" s="4">
         <v>4</v>
@@ -3920,10 +3208,10 @@
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="1" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C4" s="4">
         <v>0.8</v>
@@ -3967,10 +3255,10 @@
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="1" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="B5" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="C5" s="4">
         <f>C6*8</f>
@@ -4015,10 +3303,10 @@
     </row>
     <row r="6" spans="1:12">
       <c r="A6" s="1" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="B6" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="C6" s="4">
         <v>1</v>
@@ -4062,10 +3350,10 @@
     </row>
     <row r="7" spans="1:12">
       <c r="A7" s="1" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="B7" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="C7" s="4">
         <v>10000</v>
@@ -4109,10 +3397,10 @@
     </row>
     <row r="8" spans="1:12">
       <c r="A8" s="1" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="B8" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="C8" s="4">
         <v>10</v>
@@ -4156,10 +3444,10 @@
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="1" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C9" s="4">
         <v>2</v>
@@ -4203,10 +3491,10 @@
     </row>
     <row r="10" spans="1:12">
       <c r="A10" s="1" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C10" s="4">
         <v>0.12</v>
@@ -4250,10 +3538,10 @@
     </row>
     <row r="11" spans="1:12">
       <c r="A11" s="1" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="B11" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C11" s="6">
         <v>31</v>
@@ -4288,10 +3576,10 @@
     </row>
     <row r="12" spans="1:12">
       <c r="A12" s="7" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="B12" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="C12" s="6">
         <v>50</v>
@@ -4335,10 +3623,10 @@
     </row>
     <row r="13" spans="1:12">
       <c r="A13" s="7" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="B13" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="C13" s="6">
         <v>60</v>
@@ -4381,7 +3669,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4403,33 +3691,33 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="H1" s="14" t="s">
-        <v>80</v>
+        <v>68</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="B2">
         <v>20</v>
@@ -4445,12 +3733,12 @@
         <v>2</v>
       </c>
       <c r="F2" t="s">
-        <v>78</v>
-      </c>
-      <c r="G2" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="H2" s="15">
+        <v>67</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="H2" s="13">
         <v>1</v>
       </c>
     </row>
@@ -4494,7 +3782,7 @@
       <c r="D15" s="2"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>